<commit_message>
Update plots, Review presentation, Adjust report, Add benchmark with big cutoff radius
</commit_message>
<xml_diff>
--- a/sheet03/data/DanielExecutionLaptop.xlsx
+++ b/sheet03/data/DanielExecutionLaptop.xlsx
@@ -1,15 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C9358AE-CCB9-4CDF-8DA5-C8ACEE28F722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tobias\MolSimPresentation\sheet03\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894FC45E-B6AE-45A9-9250-4CDE3B88F5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -22,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ParticleContainer</t>
   </si>
@@ -42,26 +48,23 @@
     <t>LinkedCells</t>
   </si>
   <si>
-    <t>Ubuntu native</t>
+    <t xml:space="preserve">Hardware: </t>
   </si>
   <si>
-    <t xml:space="preserve">hardware: </t>
+    <t>Intel i5-10210U</t>
   </si>
   <si>
-    <t>Micro-Star International Co., Ltd. Modern 15 A10RAS</t>
+    <t>8GB RAM</t>
   </si>
   <si>
-    <t xml:space="preserve">CPU: </t>
-  </si>
-  <si>
-    <t>Intel® Core™ i5-10210U CPU @ 1.60GHz × 8</t>
+    <t>Ubuntu 22.04.3 LTS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,13 +133,27 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  </a:sysClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -144,9 +161,125 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Ubuntu native, CPU: Intel® Core™ i5-10210U CPU @ 1.60GHz × 8</a:t>
+              <a:rPr lang="de-DE" sz="2000"/>
+              <a:t>Benchmark: </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Cutoff Radius: 30, Domain: 300x300x3</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE" sz="2000"/>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1050" b="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Intel</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1050" b="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> i5-10210U 4</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1050" b="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>-Core Processor 1.6GHz (4.2GHz Turbo),8GB RAM</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1050" b="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Ubuntu 22.04.3 LTS (64bit)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -162,32 +295,59 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13061947569561344"/>
+          <c:y val="0.19317687455653884"/>
+          <c:w val="0.83080518738644704"/>
+          <c:h val="0.64762712414250312"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>DirectSum</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -212,9 +372,60 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.4207837355738606E-3"/>
+                  <c:y val="-3.8305061342163674E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$2:$D$5</c:f>
+              <c:f>Tabelle1!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -235,7 +446,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$E$2:$E$5</c:f>
+              <c:f>Tabelle1!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -254,16 +465,19 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A544-48F7-969C-3BDF9502B351}"/>
+              <c16:uniqueId val="{00000001-D022-42F5-9271-C255713B9EF8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>LinkedCells</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -288,9 +502,59 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.3489661167128873E-2"/>
+                  <c:y val="-3.9389539598948919E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$2:$D$5</c:f>
+              <c:f>Tabelle1!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -311,7 +575,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$F$2:$F$5</c:f>
+              <c:f>Tabelle1!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -330,10 +594,10 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-A544-48F7-969C-3BDF9502B351}"/>
+              <c16:uniqueId val="{00000003-D022-42F5-9271-C255713B9EF8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -345,11 +609,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1656345095"/>
-        <c:axId val="1656347143"/>
+        <c:axId val="1029325616"/>
+        <c:axId val="1030472416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1656345095"/>
+        <c:axId val="1029325616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -369,20 +633,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -403,9 +653,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Size of Container</a:t>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>#</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t>Particles [spawned in rectangles]</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -434,7 +689,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -472,15 +727,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1656347143"/>
+        <c:crossAx val="1030472416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1656347143"/>
+        <c:axId val="1030472416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,8 +775,12 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>time in seconds</a:t>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t>Simulation Time </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>[s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -551,7 +810,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -589,10 +848,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1656345095"/>
+        <c:crossAx val="1029325616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -631,12 +890,19 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -661,12 +927,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1232,27 +1498,29 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219199</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>272024</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>187778</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Diagramm 4">
+        <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E699C11-A07E-5F57-2242-42F71B10F0FC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE2D550E-486D-41F1-BCC4-0551FAD0ACFE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1269,8 +1537,77 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="ManuelExecutionPC"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>DirectSum</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>LinkedCells</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>1000</v>
+          </cell>
+          <cell r="B2">
+            <v>34.664000000000001</v>
+          </cell>
+          <cell r="C2">
+            <v>29.16</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>2000</v>
+          </cell>
+          <cell r="B3">
+            <v>145.53</v>
+          </cell>
+          <cell r="C3">
+            <v>103.459</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>4000</v>
+          </cell>
+          <cell r="B4">
+            <v>619.90700000000004</v>
+          </cell>
+          <cell r="C4">
+            <v>226.739</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>8000</v>
+          </cell>
+          <cell r="B5">
+            <v>2358.1439999999998</v>
+          </cell>
+          <cell r="C5">
+            <v>430.113</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1566,84 +1903,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D1:P5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:16">
-      <c r="D1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="P1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="4:16">
-      <c r="D2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1000</v>
       </c>
-      <c r="E2" s="1">
+      <c r="B2" s="1">
         <v>20.657</v>
       </c>
-      <c r="F2" s="1">
+      <c r="C2" s="1">
         <v>12.351000000000001</v>
       </c>
     </row>
-    <row r="3" spans="4:16">
-      <c r="D3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2000</v>
       </c>
-      <c r="E3" s="1">
+      <c r="B3" s="1">
         <v>82.703999999999994</v>
       </c>
-      <c r="F3" s="1">
+      <c r="C3" s="1">
         <v>38.768999999999998</v>
       </c>
     </row>
-    <row r="4" spans="4:16">
-      <c r="D4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>4000</v>
       </c>
-      <c r="E4" s="1">
+      <c r="B4" s="1">
         <v>330.33600000000001</v>
       </c>
-      <c r="F4" s="1">
+      <c r="C4" s="1">
         <v>88.203000000000003</v>
       </c>
     </row>
-    <row r="5" spans="4:16">
-      <c r="D5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>8000</v>
       </c>
-      <c r="E5" s="1">
+      <c r="B5" s="1">
         <v>1322.912</v>
       </c>
-      <c r="F5">
+      <c r="C5">
         <v>200.66499999999999</v>
       </c>
     </row>

</xml_diff>